<commit_message>
Changed fuel types to string ID.
</commit_message>
<xml_diff>
--- a/library/data/Fuel.xlsx
+++ b/library/data/Fuel.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,18 +22,16 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author> </author>
+    <author>Unknown Author</author>
   </authors>
   <commentList>
     <comment ref="E7" authorId="0">
       <text>
         <r>
           <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
+            <sz val="10"/>
+            <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">50.8% carbon by weight, 8300 BTU/lb, offset for decay = 1.2% / year * 20 years</t>
         </r>
@@ -43,11 +41,9 @@
       <text>
         <r>
           <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
+            <sz val="10"/>
+            <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">52.9% carbon, 9000 BTU/lb, decay offset = 1.2% / year * 20 years</t>
         </r>
@@ -57,11 +53,9 @@
       <text>
         <r>
           <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
+            <sz val="10"/>
+            <rFont val="Arial"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Birch figures, but 70% decay offset since mostly comes from wood waste.</t>
         </r>
@@ -72,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="55">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -98,6 +92,9 @@
     <t xml:space="preserve">effic_choices</t>
   </si>
   <si>
+    <t xml:space="preserve">elec</t>
+  </si>
+  <si>
     <t xml:space="preserve">Electricity</t>
   </si>
   <si>
@@ -107,6 +104,9 @@
     <t xml:space="preserve">[('Electric Resistance 100%', 100)]</t>
   </si>
   <si>
+    <t xml:space="preserve">ng</t>
+  </si>
+  <si>
     <t xml:space="preserve">Natural Gas</t>
   </si>
   <si>
@@ -119,6 +119,9 @@
     <t xml:space="preserve">[('Low 74%', 74), ('Standard 80%', 80), ('High Efficiency Condensing 95%', 95)]</t>
   </si>
   <si>
+    <t xml:space="preserve">propane</t>
+  </si>
+  <si>
     <t xml:space="preserve">Propane</t>
   </si>
   <si>
@@ -128,6 +131,9 @@
     <t xml:space="preserve">PropanePrice</t>
   </si>
   <si>
+    <t xml:space="preserve">oil1</t>
+  </si>
+  <si>
     <t xml:space="preserve">#1 Oil</t>
   </si>
   <si>
@@ -137,6 +143,9 @@
     <t xml:space="preserve">[('Low 74%', 74), ('Standard 80%', 80), ('High Efficiency (e.g. Toyostove) 84%', 84)]</t>
   </si>
   <si>
+    <t xml:space="preserve">oil2</t>
+  </si>
+  <si>
     <t xml:space="preserve">#2 Oil</t>
   </si>
   <si>
@@ -146,6 +155,9 @@
     <t xml:space="preserve">[('Low 74%', 74), ('Standard 80%', 80), ('High Efficiency 84%', 84)]</t>
   </si>
   <si>
+    <t xml:space="preserve">birch</t>
+  </si>
+  <si>
     <t xml:space="preserve">Birch Wood</t>
   </si>
   <si>
@@ -158,12 +170,18 @@
     <t xml:space="preserve">[('Standard 50%', 50), ('Catalytic 60%', 60)]</t>
   </si>
   <si>
+    <t xml:space="preserve">spruce</t>
+  </si>
+  <si>
     <t xml:space="preserve">Spruce Wood</t>
   </si>
   <si>
     <t xml:space="preserve">SprucePrice</t>
   </si>
   <si>
+    <t xml:space="preserve">pellets</t>
+  </si>
+  <si>
     <t xml:space="preserve">Wood Pellets</t>
   </si>
   <si>
@@ -176,6 +194,9 @@
     <t xml:space="preserve">[('Standard 70%', 70), ('High Efficiency 75%', 75)]</t>
   </si>
   <si>
+    <t xml:space="preserve">coal</t>
+  </si>
+  <si>
     <t xml:space="preserve">Coal</t>
   </si>
   <si>
@@ -185,6 +206,9 @@
     <t xml:space="preserve">[('Standard 60%', 60)]</t>
   </si>
   <si>
+    <t xml:space="preserve">steam</t>
+  </si>
+  <si>
     <t xml:space="preserve">District Heat, Steam</t>
   </si>
   <si>
@@ -195,6 +219,9 @@
   </si>
   <si>
     <t xml:space="preserve">[('Standard 99%', 99)]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hot_water</t>
   </si>
   <si>
     <t xml:space="preserve">District Heat, Hot Water</t>
@@ -216,7 +243,7 @@
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
     <numFmt numFmtId="167" formatCode="#,##0.00"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -247,6 +274,11 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -302,67 +334,67 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -378,18 +410,124 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="22.3"/>
@@ -428,14 +566,14 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="12" t="n">
-        <v>1</v>
+      <c r="A2" s="12" t="s">
+        <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" s="13" t="n">
         <v>3413</v>
@@ -445,18 +583,18 @@
         <v>0.93</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="12" t="n">
-        <v>2</v>
+      <c r="A3" s="12" t="s">
+        <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D3" s="13" t="n">
         <v>103700</v>
@@ -465,24 +603,24 @@
         <v>117</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G3" s="15" t="n">
         <v>0.58</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12" t="n">
-        <v>3</v>
+      <c r="A4" s="12" t="s">
+        <v>17</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D4" s="13" t="n">
         <v>91333</v>
@@ -491,24 +629,24 @@
         <v>139</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G4" s="15" t="n">
         <v>0.58</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="12" t="n">
-        <v>4</v>
+      <c r="A5" s="12" t="s">
+        <v>21</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D5" s="13" t="n">
         <v>137452</v>
@@ -517,24 +655,24 @@
         <v>161.3</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="G5" s="15" t="n">
         <v>0.6</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="12" t="n">
-        <v>5</v>
+      <c r="A6" s="12" t="s">
+        <v>25</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D6" s="13" t="n">
         <v>138500</v>
@@ -543,24 +681,24 @@
         <v>161.3</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="G6" s="15" t="n">
         <v>0.6</v>
       </c>
       <c r="H6" s="16" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="12" t="n">
-        <v>6</v>
+      <c r="A7" s="12" t="s">
+        <v>29</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D7" s="13" t="n">
         <v>23600000</v>
@@ -569,24 +707,24 @@
         <v>171</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="G7" s="15" t="n">
         <v>0.5</v>
       </c>
       <c r="H7" s="16" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="12" t="n">
-        <v>7</v>
+      <c r="A8" s="12" t="s">
+        <v>34</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D8" s="13" t="n">
         <v>18100000</v>
@@ -595,24 +733,24 @@
         <v>164</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="G8" s="15" t="n">
         <v>0.5</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="12" t="n">
-        <v>8</v>
+      <c r="A9" s="12" t="s">
+        <v>37</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="D9" s="13" t="n">
         <v>16000000</v>
@@ -621,24 +759,24 @@
         <v>67</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="G9" s="15" t="n">
         <v>0.55</v>
       </c>
       <c r="H9" s="16" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="12" t="n">
-        <v>9</v>
+      <c r="A10" s="12" t="s">
+        <v>42</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="D10" s="13" t="n">
         <v>17400000</v>
@@ -647,24 +785,24 @@
         <v>210.2</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="G10" s="15" t="n">
         <v>0.5</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="12" t="n">
-        <v>10</v>
+      <c r="A11" s="12" t="s">
+        <v>46</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="D11" s="13" t="n">
         <v>960000</v>
@@ -673,24 +811,24 @@
         <v>58</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="G11" s="15" t="n">
         <v>0.94</v>
       </c>
       <c r="H11" s="16" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="12" t="n">
-        <v>11</v>
+      <c r="A12" s="12" t="s">
+        <v>51</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="D12" s="13" t="n">
         <v>1000000</v>
@@ -699,13 +837,13 @@
         <v>58</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="G12" s="15" t="n">
         <v>0.94</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed Units and CO2 for Wood Pellets fuel type.
</commit_message>
<xml_diff>
--- a/library/data/Fuel.xlsx
+++ b/library/data/Fuel.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,16 +22,60 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author>Unknown Author</author>
+    <author> </author>
   </authors>
   <commentList>
+    <comment ref="D1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">BTUs per Fuel Unit (e.g. gallon)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">ChatGPT says 8000 – 8600 BTU / lb</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Pounds / MMBTU</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="E7" authorId="0">
       <text>
         <r>
           <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">50.8% carbon by weight, 8300 BTU/lb, offset for decay = 1.2% / year * 20 years</t>
         </r>
@@ -41,9 +85,11 @@
       <text>
         <r>
           <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">52.9% carbon, 9000 BTU/lb, decay offset = 1.2% / year * 20 years</t>
         </r>
@@ -53,11 +99,13 @@
       <text>
         <r>
           <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Birch figures, but 70% decay offset since mostly comes from wood waste.</t>
+          <t xml:space="preserve">7% moisture content (based on dry weight). 0.508 lb Carbon per lb dry wood. 70% decay offset.</t>
         </r>
       </text>
     </comment>
@@ -66,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="56">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -185,19 +233,22 @@
     <t xml:space="preserve">Wood Pellets</t>
   </si>
   <si>
+    <t xml:space="preserve">pound</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WoodPelletsPrice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[('Standard 70%', 70), ('High Efficiency 75%', 75)]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coal</t>
+  </si>
+  <si>
     <t xml:space="preserve">ton</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WoodPelletsPrice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[('Standard 70%', 70), ('High Efficiency 75%', 75)]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">coal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coal</t>
   </si>
   <si>
     <t xml:space="preserve">CoalPrice</t>
@@ -243,7 +294,7 @@
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
     <numFmt numFmtId="167" formatCode="#,##0.00"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -274,11 +325,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -410,121 +456,15 @@
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
-  <a:themeElements>
-    <a:clrScheme name="LibreOffice">
-      <a:dk1>
-        <a:srgbClr val="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:srgbClr val="ffffff"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="000000"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="ffffff"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="18a303"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="0369a3"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="a33e03"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8e03a3"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="c99c00"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="c9211e"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000ee"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="551a8b"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme>
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -753,10 +693,10 @@
         <v>39</v>
       </c>
       <c r="D9" s="13" t="n">
-        <v>16000000</v>
+        <v>8300</v>
       </c>
       <c r="E9" s="14" t="n">
-        <v>67</v>
+        <v>62.9</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>40</v>
@@ -776,7 +716,7 @@
         <v>43</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="D10" s="13" t="n">
         <v>17400000</v>
@@ -785,24 +725,24 @@
         <v>210.2</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G10" s="15" t="n">
         <v>0.5</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D11" s="13" t="n">
         <v>960000</v>
@@ -811,24 +751,24 @@
         <v>58</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G11" s="15" t="n">
         <v>0.94</v>
       </c>
       <c r="H11" s="16" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="12" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D12" s="13" t="n">
         <v>1000000</v>
@@ -837,13 +777,13 @@
         <v>58</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G12" s="15" t="n">
         <v>0.94</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>